<commit_message>
Exploring and using Plaque half life or time-double Same equation same math
</commit_message>
<xml_diff>
--- a/Analysis/BasicStatisticsOfClearly-Keto-CTA_dataAndRegressionMining.xlsx
+++ b/Analysis/BasicStatisticsOfClearly-Keto-CTA_dataAndRegressionMining.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jille\source\repos\NinerXrayBravoTwoTwo\Keto_Cta\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E36F02-5FA4-41C2-93E3-E9CE01DAEBC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC65C69-2761-4B0C-B0E9-2EA45E4343CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="360" windowWidth="23256" windowHeight="13896" xr2:uid="{D0CD085A-3F8F-465F-9DED-72CF3944BED2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{D0CD085A-3F8F-465F-9DED-72CF3944BED2}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Stats" sheetId="1" r:id="rId1"/>
@@ -11940,7 +11940,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{708365D3-941B-4509-BD95-53FBCFEAE097}">
   <dimension ref="A1:AG50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="Y28" sqref="Y28"/>
     </sheetView>
   </sheetViews>

</xml_diff>